<commit_message>
bis dash board added
bis dash board added
</commit_message>
<xml_diff>
--- a/TT231_DemoScreen_work_Status.xlsx
+++ b/TT231_DemoScreen_work_Status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14220" windowHeight="6030" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14220" windowHeight="6036" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Screens" sheetId="3" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="469">
   <si>
     <t>Notes</t>
   </si>
@@ -1361,48 +1361,6 @@
     <t>&gt;60 expressway - green</t>
   </si>
   <si>
-    <r>
-      <t>dark </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF222222"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>green</t>
-    </r>
-  </si>
-  <si>
-    <t>#006400</t>
-  </si>
-  <si>
-    <t>#ffbf00</t>
-  </si>
-  <si>
-    <t>amber</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>#FF0000</t>
-  </si>
-  <si>
-    <t>Dark Red</t>
-  </si>
-  <si>
-    <t>#8b0000</t>
-  </si>
-  <si>
-    <t>Green</t>
-  </si>
-  <si>
-    <t>#00FF00</t>
-  </si>
-  <si>
     <t>The csv Speed data file is not import proberly</t>
   </si>
   <si>
@@ -1437,6 +1395,114 @@
   </si>
   <si>
     <t>if call the new layer, existing layer has to be deleted.</t>
+  </si>
+  <si>
+    <t>8/7 - 12/7</t>
+  </si>
+  <si>
+    <t>BIS Part - Speed data chart, Incident data Chart</t>
+  </si>
+  <si>
+    <t>Zone selection page removed, Login and command control page linked</t>
+  </si>
+  <si>
+    <t>Change the font color in command control</t>
+  </si>
+  <si>
+    <t>Working on LTA Feedback</t>
+  </si>
+  <si>
+    <t>Draw prediction on map after creating accident</t>
+  </si>
+  <si>
+    <t>75,175,198 - blue</t>
+  </si>
+  <si>
+    <t>192,80,77 - brown</t>
+  </si>
+  <si>
+    <t>155,187,89 - green</t>
+  </si>
+  <si>
+    <t>128,100,162 - lavender</t>
+  </si>
+  <si>
+    <t>79,129,189 - dark blue</t>
+  </si>
+  <si>
+    <t>0,176,80 - green</t>
+  </si>
+  <si>
+    <t>192,0,0 - red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">255, 192, 0 - yellow </t>
+  </si>
+  <si>
+    <t>219,132,61 - brown</t>
+  </si>
+  <si>
+    <t>170, 70, 67 - burgundy</t>
+  </si>
+  <si>
+    <t>#006400 - dark green</t>
+  </si>
+  <si>
+    <t>#ffbf00 - amber</t>
+  </si>
+  <si>
+    <t>#FF0000 - red</t>
+  </si>
+  <si>
+    <t>#8b0000 - Dark Red</t>
+  </si>
+  <si>
+    <t>#00FF00 - Green</t>
+  </si>
+  <si>
+    <t>#ffffff - white</t>
+  </si>
+  <si>
+    <t>#000000 - Black</t>
+  </si>
+  <si>
+    <t>eqt_id - sapsc_719085, sapsc_719084, sapsc_719082</t>
+  </si>
+  <si>
+    <t>CCTV Camera Location</t>
+  </si>
+  <si>
+    <t>103.8587667</t>
+  </si>
+  <si>
+    <t>1.3752537</t>
+  </si>
+  <si>
+    <t>103.8582773</t>
+  </si>
+  <si>
+    <t>1.3770134</t>
+  </si>
+  <si>
+    <t>103.8584744</t>
+  </si>
+  <si>
+    <t>1.3778264</t>
+  </si>
+  <si>
+    <t>Camera Points added on the map</t>
+  </si>
+  <si>
+    <t>Video generated based on the camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new traffic speed layer added near the accident location </t>
+  </si>
+  <si>
+    <t>bis module json file added</t>
+  </si>
+  <si>
+    <t>changing the bis format as per new ppt (Infographics_conclusion_v5 (with comments))</t>
   </si>
 </sst>
 </file>
@@ -1650,19 +1716,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3" tint="-0.499984740745262"/>
@@ -1680,6 +1733,20 @@
       <color rgb="FF202124"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1997,35 +2064,35 @@
     <xf numFmtId="17" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="29" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="17" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -2332,8 +2399,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>206169</xdr:rowOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>429</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2758,6 +2825,87 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3223540</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>99244</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5524500"/>
+          <a:ext cx="3223540" cy="2126164"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3002531</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>38282</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="106680" y="7764780"/>
+          <a:ext cx="2895851" cy="2103302"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="ProjectTracker3" displayName="ProjectTracker3" ref="A3:H29" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8" headerRowCellStyle="Heading 2">
   <autoFilter ref="A3:H29"/>
@@ -3031,27 +3179,27 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.25" customWidth="1"/>
-    <col min="2" max="2" width="22.625" customWidth="1"/>
-    <col min="3" max="3" width="16.875" customWidth="1"/>
+    <col min="1" max="1" width="23.19921875" customWidth="1"/>
+    <col min="2" max="2" width="22.59765625" customWidth="1"/>
+    <col min="3" max="3" width="16.8984375" customWidth="1"/>
     <col min="4" max="4" width="50.5" style="17" customWidth="1"/>
     <col min="5" max="5" width="21.5" style="5" customWidth="1"/>
-    <col min="6" max="6" width="16.125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.375" customWidth="1"/>
-    <col min="8" max="8" width="16.375" customWidth="1"/>
+    <col min="6" max="6" width="16.09765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.3984375" customWidth="1"/>
+    <col min="8" max="8" width="16.3984375" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:8" s="10" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -3077,7 +3225,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -3099,7 +3247,7 @@
       </c>
       <c r="H4" s="20"/>
     </row>
-    <row r="5" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -3121,7 +3269,7 @@
       </c>
       <c r="H5" s="20"/>
     </row>
-    <row r="6" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
@@ -3145,7 +3293,7 @@
       </c>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>15</v>
       </c>
@@ -3167,7 +3315,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -3189,7 +3337,7 @@
       </c>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>15</v>
       </c>
@@ -3211,7 +3359,7 @@
       </c>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>15</v>
       </c>
@@ -3233,7 +3381,7 @@
       </c>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>15</v>
       </c>
@@ -3255,7 +3403,7 @@
       </c>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
@@ -3277,7 +3425,7 @@
       </c>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:8" s="10" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" s="10" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -3301,7 +3449,7 @@
       </c>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>15</v>
       </c>
@@ -3325,7 +3473,7 @@
       </c>
       <c r="H14" s="20"/>
     </row>
-    <row r="15" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="11" t="s">
         <v>51</v>
@@ -3347,7 +3495,7 @@
       </c>
       <c r="H15" s="20"/>
     </row>
-    <row r="16" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="11" t="s">
         <v>59</v>
@@ -3371,7 +3519,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="11" t="s">
         <v>59</v>
@@ -3391,7 +3539,7 @@
       </c>
       <c r="H17" s="20"/>
     </row>
-    <row r="18" spans="1:8" s="10" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="10" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>65</v>
       </c>
@@ -3407,7 +3555,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>68</v>
       </c>
@@ -3429,7 +3577,7 @@
       <c r="G19" s="16"/>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="11" t="s">
         <v>75</v>
@@ -3451,7 +3599,7 @@
       </c>
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="11" t="s">
         <v>82</v>
@@ -3473,7 +3621,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="11" t="s">
         <v>86</v>
@@ -3493,7 +3641,7 @@
       <c r="G22" s="16"/>
       <c r="H22" s="20"/>
     </row>
-    <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="11" t="s">
         <v>93</v>
@@ -3513,7 +3661,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="20"/>
     </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="11" t="s">
         <v>96</v>
@@ -3533,7 +3681,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="20"/>
     </row>
-    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="11" t="s">
         <v>101</v>
@@ -3553,7 +3701,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="11" t="s">
@@ -3571,7 +3719,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="11" t="s">
         <v>112</v>
@@ -3591,7 +3739,7 @@
       <c r="G27" s="16"/>
       <c r="H27" s="20"/>
     </row>
-    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="11" t="s">
         <v>115</v>
@@ -3609,7 +3757,7 @@
       <c r="G28" s="16"/>
       <c r="H28" s="20"/>
     </row>
-    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -3651,36 +3799,36 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.125" customWidth="1"/>
-    <col min="3" max="3" width="31.625" customWidth="1"/>
+    <col min="2" max="2" width="13.09765625" customWidth="1"/>
+    <col min="3" max="3" width="31.59765625" customWidth="1"/>
     <col min="4" max="4" width="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="44"/>
       <c r="D1" s="44"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D2" s="44"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="D3" s="44"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B79" s="44"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B82" s="45"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B86" s="44"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B90" s="44"/>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B93" s="44"/>
     </row>
   </sheetData>
@@ -3702,41 +3850,41 @@
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66.625" customWidth="1"/>
+    <col min="1" max="1" width="66.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
     </row>
   </sheetData>
@@ -3761,17 +3909,17 @@
       <selection pane="bottomLeft" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="24.25" customWidth="1"/>
+    <col min="2" max="2" width="24.19921875" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="37.125" style="33" customWidth="1"/>
-    <col min="5" max="5" width="44.625" style="33" customWidth="1"/>
-    <col min="6" max="6" width="59.625" customWidth="1"/>
+    <col min="4" max="4" width="37.09765625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="44.59765625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="59.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>131</v>
       </c>
@@ -3791,7 +3939,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
@@ -3805,7 +3953,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>124</v>
       </c>
@@ -3816,7 +3964,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>132</v>
       </c>
@@ -3833,47 +3981,47 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E5" s="33" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="E6" s="33" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
       <c r="E7" s="33" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E8" s="33" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="34" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" s="35" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E11" s="35" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>137</v>
       </c>
@@ -3887,7 +4035,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>138</v>
       </c>
@@ -3895,27 +4043,27 @@
         <v>142</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E21" s="33" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E23" s="32" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E24" s="33" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
       <c r="E25" s="33" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
         <v>148</v>
       </c>
@@ -3923,27 +4071,27 @@
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E32" s="33" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E33" s="33" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E34" s="33" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E35" s="33" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>165</v>
       </c>
@@ -3960,7 +4108,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>164</v>
       </c>
@@ -3974,7 +4122,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>169</v>
       </c>
@@ -3985,7 +4133,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>171</v>
       </c>
@@ -3993,7 +4141,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>175</v>
       </c>
@@ -4001,7 +4149,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>173</v>
       </c>
@@ -4012,7 +4160,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>214</v>
       </c>
@@ -4023,7 +4171,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>215</v>
       </c>
@@ -4031,7 +4179,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
         <v>170</v>
       </c>
@@ -4042,7 +4190,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="24"/>
       <c r="C49" t="s">
         <v>173</v>
@@ -4051,7 +4199,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="24"/>
       <c r="C50" t="s">
         <v>168</v>
@@ -4060,7 +4208,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="24"/>
       <c r="C51" t="s">
         <v>221</v>
@@ -4069,13 +4217,13 @@
         <v>216</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="24"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="24"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>38</v>
       </c>
@@ -4086,7 +4234,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
         <v>173</v>
       </c>
@@ -4094,7 +4242,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
         <v>168</v>
       </c>
@@ -4105,7 +4253,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="33" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>189</v>
       </c>
@@ -4116,7 +4264,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>197</v>
       </c>
@@ -4124,12 +4272,12 @@
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E60" s="33" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E61" s="33" t="s">
         <v>194</v>
       </c>
@@ -4146,23 +4294,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G96"/>
+  <dimension ref="A1:G107"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+      <selection activeCell="B100" sqref="B100:B107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="28" customWidth="1"/>
-    <col min="2" max="2" width="20.75" style="42" customWidth="1"/>
-    <col min="3" max="3" width="14.75" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="2" max="2" width="20.69921875" style="42" customWidth="1"/>
+    <col min="3" max="3" width="14.69921875" customWidth="1"/>
+    <col min="4" max="4" width="7.09765625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="7" max="7" width="34.875" customWidth="1"/>
+    <col min="7" max="7" width="34.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>155</v>
       </c>
@@ -4176,7 +4324,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="28">
         <v>103.839</v>
       </c>
@@ -4190,7 +4338,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="29">
         <v>103.81699999999999</v>
       </c>
@@ -4201,7 +4349,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="28">
         <v>103.806</v>
       </c>
@@ -4212,7 +4360,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>103.79</v>
       </c>
@@ -4223,7 +4371,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="28">
         <v>103.77800000000001</v>
       </c>
@@ -4234,21 +4382,21 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="43"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E10" s="24" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <v>103.884</v>
       </c>
@@ -4259,7 +4407,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <v>103.851</v>
       </c>
@@ -4270,28 +4418,28 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>203</v>
       </c>
       <c r="E14" s="30"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="28">
         <v>103.839</v>
       </c>
@@ -4302,7 +4450,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="29">
         <v>103.81699999999999</v>
       </c>
@@ -4313,7 +4461,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="28">
         <v>103.806</v>
       </c>
@@ -4324,42 +4472,42 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E24" s="24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="28">
         <v>103.79</v>
       </c>
@@ -4370,7 +4518,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="28">
         <v>103.77800000000001</v>
       </c>
@@ -4381,17 +4529,17 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
         <v>237</v>
       </c>
@@ -4402,7 +4550,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>236</v>
       </c>
@@ -4413,7 +4561,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="28">
         <v>1.332525</v>
       </c>
@@ -4424,7 +4572,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="28">
         <v>1.331914</v>
       </c>
@@ -4435,7 +4583,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
         <v>243</v>
       </c>
@@ -4446,7 +4594,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="28">
         <v>103.857499</v>
       </c>
@@ -4460,7 +4608,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="28">
         <v>103.8581903</v>
       </c>
@@ -4468,7 +4616,7 @@
         <v>1.3837919999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="28">
         <v>103.8553513</v>
       </c>
@@ -4476,7 +4624,7 @@
         <v>1.3759417</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="28">
         <v>103.8583969</v>
       </c>
@@ -4484,12 +4632,12 @@
         <v>1.3615294</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" s="42" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
         <v>265</v>
       </c>
@@ -4503,7 +4651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>266</v>
       </c>
@@ -4514,7 +4662,7 @@
         <v>1.3759417</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
         <v>265</v>
       </c>
@@ -4528,7 +4676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>266</v>
       </c>
@@ -4539,7 +4687,7 @@
         <v>1.3777482999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
         <v>265</v>
       </c>
@@ -4553,7 +4701,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
         <v>266</v>
       </c>
@@ -4564,7 +4712,7 @@
         <v>1.3705164999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
         <v>265</v>
       </c>
@@ -4578,7 +4726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="28" t="s">
         <v>266</v>
       </c>
@@ -4589,7 +4737,7 @@
         <v>1.3691533</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="28" t="s">
         <v>265</v>
       </c>
@@ -4603,7 +4751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="28" t="s">
         <v>266</v>
       </c>
@@ -4614,7 +4762,7 @@
         <v>1.3627773000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="28" t="s">
         <v>265</v>
       </c>
@@ -4628,7 +4776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="28" t="s">
         <v>266</v>
       </c>
@@ -4639,7 +4787,7 @@
         <v>1.3615294</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="28" t="s">
         <v>265</v>
       </c>
@@ -4653,7 +4801,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="28" t="s">
         <v>266</v>
       </c>
@@ -4664,7 +4812,7 @@
         <v>1.3837919999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="28" t="s">
         <v>265</v>
       </c>
@@ -4678,7 +4826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="28" t="s">
         <v>266</v>
       </c>
@@ -4689,7 +4837,7 @@
         <v>1.3855739</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="28" t="s">
         <v>386</v>
       </c>
@@ -4697,57 +4845,57 @@
         <v>387</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="28" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="28" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="28" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="28" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="28" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="28" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="28" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="28" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="28" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="28">
         <v>1471</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="28">
         <v>31088.9</v>
       </c>
@@ -4755,7 +4903,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="28">
         <v>39920.080000000002</v>
       </c>
@@ -4763,12 +4911,12 @@
         <v>391</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="28">
         <v>426</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="28">
         <v>30755.81</v>
       </c>
@@ -4776,7 +4924,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="28">
         <v>39822.019999999997</v>
       </c>
@@ -4784,12 +4932,12 @@
         <v>393</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="28">
         <v>1270</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="28">
         <v>30383.93</v>
       </c>
@@ -4797,12 +4945,70 @@
         <v>394</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="28">
         <v>39757.74</v>
       </c>
       <c r="B96" s="42" t="s">
         <v>395</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="28" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>30832.0437322</v>
+      </c>
+      <c r="B100" s="42" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>39694.078958400001</v>
+      </c>
+      <c r="B101" s="42" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>30777.594452199999</v>
+      </c>
+      <c r="B103" s="42" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>39888.679278600001</v>
+      </c>
+      <c r="B104" s="42" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>30799.527124200002</v>
+      </c>
+      <c r="B106" s="42" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>39978.569966700001</v>
+      </c>
+      <c r="B107" s="42" t="s">
+        <v>463</v>
       </c>
     </row>
   </sheetData>
@@ -4823,63 +5029,63 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.625" style="33" customWidth="1"/>
-    <col min="2" max="2" width="57.875" customWidth="1"/>
+    <col min="1" max="1" width="48.59765625" style="33" customWidth="1"/>
+    <col min="2" max="2" width="57.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="33" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="32" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="33" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A56" s="33" t="s">
         <v>201</v>
       </c>
@@ -4898,13 +5104,13 @@
       <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.875" customWidth="1"/>
-    <col min="2" max="2" width="23.75" customWidth="1"/>
+    <col min="1" max="1" width="22.8984375" customWidth="1"/>
+    <col min="2" max="2" width="23.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>222</v>
       </c>
@@ -4923,14 +5129,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.5" customWidth="1"/>
     <col min="2" max="2" width="26.5" customWidth="1"/>
-    <col min="3" max="3" width="71.625" customWidth="1"/>
+    <col min="3" max="3" width="71.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>223</v>
       </c>
@@ -4941,7 +5147,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
         <v>226</v>
       </c>
@@ -4952,7 +5158,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
         <v>228</v>
       </c>
@@ -4963,20 +5169,20 @@
         <v>230</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="38"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="39" t="s">
         <v>247</v>
       </c>
@@ -4992,609 +5198,660 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C111" sqref="C111"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.125" style="50" customWidth="1"/>
-    <col min="2" max="2" width="28.125" style="50" customWidth="1"/>
-    <col min="3" max="3" width="106.875" style="50" customWidth="1"/>
-    <col min="4" max="16384" width="8.75" style="50"/>
+    <col min="1" max="1" width="12.09765625" style="47" customWidth="1"/>
+    <col min="2" max="2" width="28.09765625" style="47" customWidth="1"/>
+    <col min="3" max="3" width="106.8984375" style="47" customWidth="1"/>
+    <col min="4" max="16384" width="8.69921875" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="46" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="46" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
         <v>337</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="47" t="s">
         <v>353</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="51" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C3" s="54" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="51" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C4" s="54" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="51" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C5" s="54"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="53" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="51"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="50" t="s">
         <v>338</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="51" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C7" s="54" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="51" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="50" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
         <v>340</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="51" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C10" s="54" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="51" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C11" s="54" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="51" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="55"/>
-      <c r="C12" s="54" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="52"/>
+      <c r="C12" s="51" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C13" s="54" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="51" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C14" s="54" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="51" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C15" s="54" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="51" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C16" s="54"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="50" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="51"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="47" t="s">
         <v>345</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="51" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="54" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="51" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C19" s="54" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="51" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C20" s="54" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="51" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C21" s="54" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="51" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="50" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="47" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="50" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="47" t="s">
         <v>347</v>
       </c>
-      <c r="C24" s="54" t="s">
+      <c r="C24" s="51" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C25" s="54" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="51" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="55"/>
-      <c r="C26" s="54" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="52"/>
+      <c r="C26" s="51" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C27" s="54" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="51" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C28" s="54" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="51" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="50" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="47" t="s">
         <v>350</v>
       </c>
-      <c r="C30" s="54" t="s">
+      <c r="C30" s="51" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C31" s="54" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="51" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C32" s="54" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="51" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="54"/>
-      <c r="C33" s="54" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="51"/>
+      <c r="C33" s="51" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="54" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="51" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="54" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="51" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="54" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="51" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="54" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="51" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="54" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="51" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="54" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="51" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="50" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="47" t="s">
         <v>341</v>
       </c>
-      <c r="C41" s="54" t="s">
+      <c r="C41" s="51" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="54" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="51" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C43" s="54" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="51" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C44" s="54" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="51" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C45" s="54" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="51" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="55"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="55" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="52"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="52" t="s">
         <v>342</v>
       </c>
-      <c r="C47" s="54" t="s">
+      <c r="C47" s="51" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C48" s="54" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="51" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C49" s="54" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="51" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C50" s="54" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="51" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="50" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="47" t="s">
         <v>343</v>
       </c>
-      <c r="B52" s="50" t="s">
+      <c r="B52" s="47" t="s">
         <v>360</v>
       </c>
-      <c r="C52" s="54" t="s">
+      <c r="C52" s="51" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="50" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="47" t="s">
         <v>344</v>
       </c>
-      <c r="C53" s="54" t="s">
+      <c r="C53" s="51" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="50" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="47" t="s">
         <v>359</v>
       </c>
-      <c r="C54" s="54" t="s">
+      <c r="C54" s="51" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="50" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="47" t="s">
         <v>354</v>
       </c>
-      <c r="C55" s="54" t="s">
+      <c r="C55" s="51" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="50" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="47" t="s">
         <v>355</v>
       </c>
-      <c r="C56" s="54" t="s">
+      <c r="C56" s="51" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="50" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="47" t="s">
         <v>356</v>
       </c>
-      <c r="C57" s="54" t="s">
+      <c r="C57" s="51" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="50" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="47" t="s">
         <v>357</v>
       </c>
-      <c r="C58" s="54" t="s">
+      <c r="C58" s="51" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C59" s="54" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="51" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C60" s="54" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="51" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C61" s="54" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="51" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C62" s="54" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="51" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C63" s="54" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="51" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C64" s="54" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="51" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C65" s="54" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="51" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C66" s="54" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="51" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C67" s="54" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="51" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C68" s="54" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="51" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C69" s="54" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="51" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C70" s="54"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C71" s="54"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="50" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="51"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="51"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="47" t="s">
         <v>358</v>
       </c>
-      <c r="B72" s="50" t="s">
+      <c r="B72" s="47" t="s">
         <v>290</v>
       </c>
-      <c r="C72" s="50" t="s">
+      <c r="C72" s="47" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C73" s="50" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="47" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C74" s="50" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="47" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C75" s="50" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="47" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C76" s="50" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="47" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="51" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="48" t="s">
         <v>246</v>
       </c>
-      <c r="B77" s="50" t="s">
+      <c r="B77" s="47" t="s">
         <v>259</v>
       </c>
-      <c r="C77" s="50" t="s">
+      <c r="C77" s="47" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C78" s="50" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="47" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C79" s="50" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="47" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B80" s="50" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="47" t="s">
         <v>264</v>
       </c>
-      <c r="C80" s="50" t="s">
+      <c r="C80" s="47" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C81" s="50" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="47" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C82" s="50" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="47" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C83" s="50" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="47" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C84" s="50" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="47" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="52" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="C85" s="50" t="s">
+      <c r="C85" s="47" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C86" s="50" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="47" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C87" s="50" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="47" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C88" s="50" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="47" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B89" s="50" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="47" t="s">
         <v>377</v>
       </c>
-      <c r="C89" s="50" t="s">
+      <c r="C89" s="47" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C90" s="50" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="47" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C91" s="50" t="s">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="47" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C92" s="50" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="47" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="50" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="47" t="s">
         <v>352</v>
       </c>
-      <c r="B94" s="49" t="s">
+      <c r="B94" s="46" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C95" s="50" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="47" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C96" s="50" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="47" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C97" s="50" t="s">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="47" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C98" s="50" t="s">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="47" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C99" s="50" t="s">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="47" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="47" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="47" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="47" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C112" s="47" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="47" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C114" s="47" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="47" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C116" s="47" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C117" s="47" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C118" s="47" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C100" s="50" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C119" s="47" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="101" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C101" s="50" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="47" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="111" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C111" s="50" t="s">
+      <c r="C121" s="47" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="112" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C112" s="50" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B122" s="47" t="s">
+        <v>437</v>
+      </c>
+      <c r="C122" s="47" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C113" s="50" t="s">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="47" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C114" s="50" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="115" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C115" s="50" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C124" s="47" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="116" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C116" s="50" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="117" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C117" s="50" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="118" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C118" s="50" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="119" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C119" s="50" t="s">
-        <v>442</v>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C125" s="47" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C126" s="47" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C127" s="47" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C128" s="47" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="47" t="s">
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -5606,206 +5863,241 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.5" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="46" t="s">
-        <v>421</v>
-      </c>
-      <c r="B33" s="46" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>424</v>
-      </c>
-      <c r="B34" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="47" t="s">
-        <v>425</v>
-      </c>
-      <c r="B35" s="46" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>427</v>
-      </c>
-      <c r="B36" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>429</v>
-      </c>
-      <c r="B37" s="48" t="s">
-        <v>430</v>
+    <row r="33" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="53"/>
+      <c r="B33" s="53" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="54"/>
+      <c r="B34" s="54" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="53"/>
+      <c r="B35" s="53" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="54"/>
+      <c r="B36" s="54" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="54"/>
+      <c r="B37" s="55" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>448</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e39e7e9e36de66d473ce04bb4ab2dbb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19dc5994665da46609c24125788630d8" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -6010,10 +6302,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78C4875-2E31-4ACC-AEED-0DAFD072C30B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6036,20 +6356,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78C4875-2E31-4ACC-AEED-0DAFD072C30B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
accident and mrw task
 vms images added, sce1 and sce 2
</commit_message>
<xml_diff>
--- a/TT231_DemoScreen_work_Status.xlsx
+++ b/TT231_DemoScreen_work_Status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14220" windowHeight="6036" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2160" windowHeight="1176" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Screens" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Issue facing" sheetId="10" r:id="rId9"/>
     <sheet name="Projectfilelocation" sheetId="11" r:id="rId10"/>
     <sheet name="Sheet1" sheetId="12" r:id="rId11"/>
+    <sheet name="Sheet2" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc535884" localSheetId="0">Screens!$E$19</definedName>
@@ -28,14 +29,6 @@
     <definedName name="FlagPercent">#REF!</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -96,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="607">
   <si>
     <t>Notes</t>
   </si>
@@ -1717,6 +1710,207 @@
   </si>
   <si>
     <t>Commission</t>
+  </si>
+  <si>
+    <t>29/7 - 2/8</t>
+  </si>
+  <si>
+    <t>Ccgrid view changed to new format, fourth layer changed to traffic alert layer in command control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After choose incident the traffic alert panel will open with image and video display with  map, </t>
+  </si>
+  <si>
+    <t>Speed graph created</t>
+  </si>
+  <si>
+    <t>TIP point</t>
+  </si>
+  <si>
+    <t>Event points</t>
+  </si>
+  <si>
+    <t>XY</t>
+  </si>
+  <si>
+    <t>Lati Longi</t>
+  </si>
+  <si>
+    <t>103.9459272</t>
+  </si>
+  <si>
+    <t>1.3115447</t>
+  </si>
+  <si>
+    <t>103.9374682</t>
+  </si>
+  <si>
+    <t>1.3100315</t>
+  </si>
+  <si>
+    <t>103.9276788</t>
+  </si>
+  <si>
+    <t>1.3064829</t>
+  </si>
+  <si>
+    <t>103.9236992</t>
+  </si>
+  <si>
+    <t>1.3054055</t>
+  </si>
+  <si>
+    <t>103.968971</t>
+  </si>
+  <si>
+    <t>1.3201737</t>
+  </si>
+  <si>
+    <t>103.9152873</t>
+  </si>
+  <si>
+    <t>1.3026633</t>
+  </si>
+  <si>
+    <t>103.902556</t>
+  </si>
+  <si>
+    <t>1.2987917</t>
+  </si>
+  <si>
+    <t>Detection Camera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCTV Layer </t>
+  </si>
+  <si>
+    <t>103.8610203</t>
+  </si>
+  <si>
+    <t>1.3698366</t>
+  </si>
+  <si>
+    <t>103.8587663</t>
+  </si>
+  <si>
+    <t>103.8564699</t>
+  </si>
+  <si>
+    <t>1.376076</t>
+  </si>
+  <si>
+    <t>1.3691602</t>
+  </si>
+  <si>
+    <t>103.8579652</t>
+  </si>
+  <si>
+    <t>103.8582773°</t>
+  </si>
+  <si>
+    <t>1.3770134°</t>
+  </si>
+  <si>
+    <t>103.92464</t>
+  </si>
+  <si>
+    <t>1.3113622</t>
+  </si>
+  <si>
+    <t>XY values</t>
+  </si>
+  <si>
+    <t>1.3123578</t>
+  </si>
+  <si>
+    <t>103.9237142</t>
+  </si>
+  <si>
+    <t>103.9205104</t>
+  </si>
+  <si>
+    <t>1.3113841</t>
+  </si>
+  <si>
+    <t>103.9161265</t>
+  </si>
+  <si>
+    <t>1.3097458</t>
+  </si>
+  <si>
+    <t>103.912317</t>
+  </si>
+  <si>
+    <t>1.3089701</t>
+  </si>
+  <si>
+    <t>103.8878191</t>
+  </si>
+  <si>
+    <t>1.3007663</t>
+  </si>
+  <si>
+    <t>Glide Ids Siglap Raod, East coast Road, Mountbatten Rd. for Mobile Road work</t>
+  </si>
+  <si>
+    <t>103.9246401°</t>
+  </si>
+  <si>
+    <t>1.3113624°</t>
+  </si>
+  <si>
+    <t>VMS Points in Accdient New Points inclused CTE VMS</t>
+  </si>
+  <si>
+    <t>tatip_711020</t>
+  </si>
+  <si>
+    <t>tatip_711022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIP </t>
+  </si>
+  <si>
+    <t>TSP</t>
+  </si>
+  <si>
+    <t>TTP</t>
+  </si>
+  <si>
+    <t>tcttp_713024</t>
+  </si>
+  <si>
+    <t>tcttp_713019</t>
+  </si>
+  <si>
+    <t>tatip_711018</t>
+  </si>
+  <si>
+    <t>103.8579017</t>
+  </si>
+  <si>
+    <t>1.3500895</t>
+  </si>
+  <si>
+    <t>103.8542773</t>
+  </si>
+  <si>
+    <t>1.3580211</t>
+  </si>
+  <si>
+    <t>103.8622071</t>
+  </si>
+  <si>
+    <t>1.3540672</t>
+  </si>
+  <si>
+    <t>Traffic Information Panel - traffic message (ID-start-100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Traffic Sign Panel - only sign </t>
+  </si>
+  <si>
+    <t>Traffic Time Panel - traffic message and time (ID-start-200)</t>
   </si>
 </sst>
 </file>
@@ -2151,7 +2345,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2325,6 +2519,10 @@
     </xf>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -2520,9 +2718,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleDark1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2534,10 +2729,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="127"/>
+      <c14:style val="112"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="27"/>
+      <c:style val="12"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -2614,121 +2809,121 @@
                   <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>120</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>130</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>140</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>150</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>160</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>170</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>180</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>190</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>200</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>210</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>220</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>230</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>240</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>250</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10</c:v>
+                  <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>20</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>30</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>40</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>50</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>60</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>70</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>80</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>90</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>100</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>110</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>120</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>130</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>140</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>150</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>160</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>170</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>180</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>190</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>200</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>210</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>220</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>230</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>240</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>250</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2792,121 +2987,121 @@
                   <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32000</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23000</c:v>
+                  <c:v>11.87</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24000</c:v>
+                  <c:v>12.05</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19000</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20000</c:v>
+                  <c:v>12.4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21000</c:v>
+                  <c:v>12.57</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22000</c:v>
+                  <c:v>12.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>23000</c:v>
+                  <c:v>12.99</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24000</c:v>
+                  <c:v>13.16</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>25000</c:v>
+                  <c:v>13.38</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>26000</c:v>
+                  <c:v>13.59</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27000</c:v>
+                  <c:v>13.81</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>28000</c:v>
+                  <c:v>14.03</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>29000</c:v>
+                  <c:v>14.11</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>22000</c:v>
+                  <c:v>14.21</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>23000</c:v>
+                  <c:v>14.35</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>24000</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>25000</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>21000</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>25000</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>25500</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>25700</c:v>
+                  <c:v>1.21</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>30000</c:v>
+                  <c:v>1.47</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>25200</c:v>
+                  <c:v>1.65</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>26800</c:v>
+                  <c:v>1.81</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>25400</c:v>
+                  <c:v>1.96</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>25500</c:v>
+                  <c:v>2.13</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>30000</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>25900</c:v>
+                  <c:v>2.48</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>25950</c:v>
+                  <c:v>2.64</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>25955</c:v>
+                  <c:v>2.81</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>25957</c:v>
+                  <c:v>2.92</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>25960</c:v>
+                  <c:v>3.04</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>25970</c:v>
+                  <c:v>3.05</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>26000</c:v>
+                  <c:v>3.22</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>26100</c:v>
+                  <c:v>3.38</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>26200</c:v>
+                  <c:v>3.56</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>26350</c:v>
+                  <c:v>3.73</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>26400</c:v>
+                  <c:v>3.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3017,11 +3212,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="74219008"/>
-        <c:axId val="46054144"/>
+        <c:axId val="634935808"/>
+        <c:axId val="622610112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74219008"/>
+        <c:axId val="634935808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3030,7 +3225,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46054144"/>
+        <c:crossAx val="622610112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3038,7 +3233,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46054144"/>
+        <c:axId val="622610112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3049,14 +3244,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74219008"/>
+        <c:crossAx val="634935808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3067,6 +3261,357 @@
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-SG"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$A$14:$A$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$14:$B$52</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="39"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.87</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.57</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.38</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.59</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.81</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.03</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14.21</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14.35</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.47</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.13</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.48</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.81</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.92</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.04</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.05</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.22</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.38</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.56</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.73</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.88</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="634959872"/>
+        <c:axId val="622612416"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="634959872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="622612416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="622612416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="634959872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3195,6 +3740,42 @@
         <a:xfrm>
           <a:off x="4514851" y="10058401"/>
           <a:ext cx="2381249" cy="4816268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2266951</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>261</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4019551" y="52568475"/>
+          <a:ext cx="1838324" cy="2152650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3790,6 +4371,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>209549</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4753,10 +5364,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C52"/>
+  <dimension ref="A2:C297"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4894,353 +5505,1606 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>120</v>
-      </c>
-      <c r="B14">
-        <v>32000</v>
+      <c r="A14" s="58">
+        <v>29</v>
+      </c>
+      <c r="B14" s="58">
+        <v>0</v>
       </c>
       <c r="C14">
         <v>45000</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>130</v>
-      </c>
-      <c r="B15">
-        <v>23000</v>
+      <c r="A15" s="58">
+        <v>74</v>
+      </c>
+      <c r="B15" s="58">
+        <v>11.87</v>
       </c>
       <c r="C15">
         <v>25000</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>140</v>
-      </c>
-      <c r="B16">
-        <v>24000</v>
+      <c r="A16" s="58">
+        <v>20</v>
+      </c>
+      <c r="B16" s="58">
+        <v>12.05</v>
       </c>
       <c r="C16">
         <v>30000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>150</v>
-      </c>
-      <c r="B17">
-        <v>19000</v>
+      <c r="A17" s="58">
+        <v>10</v>
+      </c>
+      <c r="B17" s="58">
+        <v>12.25</v>
       </c>
       <c r="C17">
         <v>31000</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>160</v>
-      </c>
-      <c r="B18">
-        <v>20000</v>
+      <c r="A18" s="58">
+        <v>94</v>
+      </c>
+      <c r="B18" s="58">
+        <v>12.4</v>
       </c>
       <c r="C18">
         <v>32000</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>170</v>
-      </c>
-      <c r="B19">
-        <v>21000</v>
+      <c r="A19" s="58">
+        <v>23</v>
+      </c>
+      <c r="B19" s="58">
+        <v>12.57</v>
       </c>
       <c r="C19">
         <v>33000</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>180</v>
-      </c>
-      <c r="B20">
-        <v>22000</v>
+      <c r="A20" s="58">
+        <v>62</v>
+      </c>
+      <c r="B20" s="58">
+        <v>12.75</v>
       </c>
       <c r="C20">
         <v>34000</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>190</v>
-      </c>
-      <c r="B21">
-        <v>23000</v>
+      <c r="A21" s="58">
+        <v>50</v>
+      </c>
+      <c r="B21" s="58">
+        <v>12.99</v>
       </c>
       <c r="C21">
         <v>35000</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>200</v>
-      </c>
-      <c r="B22">
-        <v>24000</v>
+      <c r="A22" s="58">
+        <v>108</v>
+      </c>
+      <c r="B22" s="58">
+        <v>13.16</v>
       </c>
       <c r="C22">
         <v>36000</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>210</v>
-      </c>
-      <c r="B23">
-        <v>25000</v>
+      <c r="A23" s="58">
+        <v>11</v>
+      </c>
+      <c r="B23" s="58">
+        <v>13.38</v>
       </c>
       <c r="C23">
         <v>30000</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>220</v>
-      </c>
-      <c r="B24">
-        <v>26000</v>
+      <c r="A24" s="58">
+        <v>12</v>
+      </c>
+      <c r="B24" s="58">
+        <v>13.59</v>
       </c>
       <c r="C24">
         <v>41000</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>230</v>
-      </c>
-      <c r="B25">
-        <v>27000</v>
+      <c r="A25" s="58">
+        <v>48</v>
+      </c>
+      <c r="B25" s="58">
+        <v>13.81</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>240</v>
-      </c>
-      <c r="B26">
-        <v>28000</v>
+      <c r="A26" s="58">
+        <v>44</v>
+      </c>
+      <c r="B26" s="58">
+        <v>14.03</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>250</v>
-      </c>
-      <c r="B27">
-        <v>29000</v>
+      <c r="A27" s="58">
+        <v>92</v>
+      </c>
+      <c r="B27" s="58">
+        <v>14.11</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="58">
+        <v>94</v>
+      </c>
+      <c r="B28" s="58">
+        <v>14.21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="58">
+        <v>97</v>
+      </c>
+      <c r="B29" s="58">
+        <v>14.35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="58">
+        <v>31</v>
+      </c>
+      <c r="B30" s="58">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="58">
+        <v>26</v>
+      </c>
+      <c r="B31" s="58">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="58">
+        <v>54</v>
+      </c>
+      <c r="B32" s="58">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="58">
+        <v>90</v>
+      </c>
+      <c r="B33" s="58">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="58">
+        <v>72</v>
+      </c>
+      <c r="B34" s="58">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="58">
+        <v>97</v>
+      </c>
+      <c r="B35" s="58">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="58">
+        <v>75</v>
+      </c>
+      <c r="B36" s="58">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="58">
+        <v>95</v>
+      </c>
+      <c r="B37" s="58">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="58">
+        <v>65</v>
+      </c>
+      <c r="B38" s="58">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="58">
+        <v>36</v>
+      </c>
+      <c r="B39" s="58">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="58">
+        <v>82</v>
+      </c>
+      <c r="B40" s="58">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="58">
+        <v>13</v>
+      </c>
+      <c r="B41" s="58">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="58">
+        <v>108</v>
+      </c>
+      <c r="B42" s="58">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="58">
+        <v>36</v>
+      </c>
+      <c r="B43" s="58">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="58">
+        <v>74</v>
+      </c>
+      <c r="B44" s="58">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="58">
+        <v>19</v>
+      </c>
+      <c r="B45" s="58">
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="58">
+        <v>75</v>
+      </c>
+      <c r="B46" s="58">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="58">
+        <v>72</v>
+      </c>
+      <c r="B47" s="58">
+        <v>3.05</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="58">
+        <v>35</v>
+      </c>
+      <c r="B48" s="58">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="58">
+        <v>65</v>
+      </c>
+      <c r="B49" s="58">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="58">
+        <v>51</v>
+      </c>
+      <c r="B50" s="58">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="58">
+        <v>25</v>
+      </c>
+      <c r="B51" s="58">
+        <v>3.73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="58">
+        <v>99</v>
+      </c>
+      <c r="B52" s="58">
+        <v>3.88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="58">
+        <v>30</v>
+      </c>
+      <c r="B53" s="58">
+        <v>4.0199999999999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="58">
+        <v>67</v>
+      </c>
+      <c r="B54" s="58">
+        <v>4.18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="58">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="58">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="58">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="58">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="58">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="58">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="58">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="58">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="58">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="58">
         <v>10</v>
       </c>
-      <c r="B28">
-        <v>22000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="58">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="58">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="58">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="58">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="58">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="58">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="58">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="58">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="58">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="58">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="58">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="58">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="58">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="58">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="58">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="58">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="58">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="58">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="58">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="58">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="58">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="58">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="58">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="58">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="58">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="58">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="58">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="58">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="58">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="58">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="58">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="58">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="58">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="58">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="58">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="58">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="58">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="58">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="58">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="58">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="58">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="58">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="58">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="58">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="58">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="58">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="58">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="58">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="58">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="58">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="58">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="58">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="58">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="58">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="58">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="58">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="58">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="58">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="58">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="58">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="58">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="58">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="58">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="58">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="58">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="58">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="58">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="58">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="58">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="58">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="58">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="58">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="58">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="58">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="58">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="58">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="58">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="58">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="58">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="58">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="58">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="58">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="58">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="58">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="58">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="58">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="58">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="58">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="58">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="58">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="58">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="58">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="58">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="58">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="58">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="58">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="58">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="58">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="58">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="58">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="58">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="58">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="58">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="58">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="58">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="58">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="58">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="58">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="58">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="58">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="58">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="58">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="58">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="58">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="58">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="58">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="58">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="58">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="58">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="58">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="58">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="58">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="58">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="58">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A200" s="58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="58">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="58">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="58">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="58">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="58">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="58">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A207" s="58">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A208" s="58">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A209" s="58">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A210" s="58">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A211" s="58">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A212" s="58">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A213" s="58">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A214" s="58">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A215" s="58">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A216" s="58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A217" s="58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A218" s="58">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A219" s="58">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A220" s="58">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A221" s="58">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A222" s="58">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A223" s="58">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A224" s="58">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A225" s="58">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A226" s="58">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A227" s="58">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A228" s="58">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A229" s="58">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A230" s="58">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A231" s="58">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A232" s="58">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A233" s="58">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A234" s="58">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A235" s="58">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A236" s="58">
         <v>20</v>
       </c>
-      <c r="B29">
-        <v>23000</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>30</v>
-      </c>
-      <c r="B30">
-        <v>24000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" s="58">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A238" s="58">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A239" s="58">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A240" s="58">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A241" s="58">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A242" s="58">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A243" s="58">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A244" s="58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A245" s="58">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A246" s="58">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A247" s="58">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A248" s="58">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A249" s="58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A250" s="58">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A251" s="58">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A252" s="58">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A253" s="58">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A254" s="58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="58">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="58">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="58">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="58">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="58">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="58">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="58">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="58">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="58">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A265" s="58">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="58">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A267" s="58">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="58">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="58">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="58">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="58">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="58">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A273" s="58">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="58">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="58">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A276" s="58">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="58">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="58">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="58">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="58">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A282" s="58">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="58">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="58">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="58">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="58">
         <v>40</v>
       </c>
-      <c r="B31">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>50</v>
-      </c>
-      <c r="B32">
-        <v>21000</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>60</v>
-      </c>
-      <c r="B33">
-        <v>25000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>70</v>
-      </c>
-      <c r="B34">
-        <v>25500</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>80</v>
-      </c>
-      <c r="B35">
-        <v>25700</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>90</v>
-      </c>
-      <c r="B36">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37">
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="58">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="58">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="58">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A290" s="58">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="58">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="58">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="58">
         <v>100</v>
       </c>
-      <c r="B37">
-        <v>25200</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>110</v>
-      </c>
-      <c r="B38">
-        <v>26800</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>120</v>
-      </c>
-      <c r="B39">
-        <v>25400</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>130</v>
-      </c>
-      <c r="B40">
-        <v>25500</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>140</v>
-      </c>
-      <c r="B41">
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>150</v>
-      </c>
-      <c r="B42">
-        <v>25900</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>160</v>
-      </c>
-      <c r="B43">
-        <v>25950</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>170</v>
-      </c>
-      <c r="B44">
-        <v>25955</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>180</v>
-      </c>
-      <c r="B45">
-        <v>25957</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>190</v>
-      </c>
-      <c r="B46">
-        <v>25960</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>200</v>
-      </c>
-      <c r="B47">
-        <v>25970</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>210</v>
-      </c>
-      <c r="B48">
-        <v>26000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>220</v>
-      </c>
-      <c r="B49">
-        <v>26100</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>230</v>
-      </c>
-      <c r="B50">
-        <v>26200</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>240</v>
-      </c>
-      <c r="B51">
-        <v>26350</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>250</v>
-      </c>
-      <c r="B52">
-        <v>26400</v>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="58">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="58">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="58">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="58">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.8984375" customWidth="1"/>
+    <col min="4" max="4" width="16.19921875" customWidth="1"/>
+    <col min="5" max="5" width="14.8984375" customWidth="1"/>
+    <col min="6" max="6" width="25.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5701,16 +7565,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G157"/>
+  <dimension ref="A1:G290"/>
   <sheetViews>
-    <sheetView topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" topLeftCell="A215" workbookViewId="0">
+      <selection activeCell="G242" sqref="G242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="28" customWidth="1"/>
-    <col min="2" max="2" width="20.69921875" style="42" customWidth="1"/>
+    <col min="2" max="2" width="50.69921875" style="42" customWidth="1"/>
     <col min="3" max="3" width="14.69921875" customWidth="1"/>
     <col min="4" max="4" width="7.09765625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
@@ -6360,17 +8224,17 @@
         <v>395</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="28" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>30832.0437322</v>
       </c>
@@ -6378,7 +8242,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>39694.078958400001</v>
       </c>
@@ -6386,7 +8250,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>30777.594452199999</v>
       </c>
@@ -6394,7 +8258,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>39888.679278600001</v>
       </c>
@@ -6402,7 +8266,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>30799.527124200002</v>
       </c>
@@ -6410,7 +8274,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>39978.569966700001</v>
       </c>
@@ -6418,261 +8282,1008 @@
         <v>463</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="28" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="28">
+        <v>38163.228498199998</v>
+      </c>
+      <c r="B110" s="42" t="s">
+        <v>573</v>
+      </c>
+      <c r="E110" s="42"/>
+      <c r="G110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="28">
+        <v>32629.488922100001</v>
+      </c>
+      <c r="B111" s="42" t="s">
+        <v>574</v>
+      </c>
+      <c r="E111" s="42"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E112" s="42"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="28">
         <v>36474.971568599998</v>
       </c>
-      <c r="B110" s="42" t="s">
+      <c r="B113" s="42" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="28">
+      <c r="E113" s="42"/>
+      <c r="G113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="28">
         <v>32287.4021058</v>
       </c>
-      <c r="B111" s="42" t="s">
+      <c r="B114" s="42" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="28">
+      <c r="E114" s="42"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E115" s="42"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="28">
         <v>36026.658896200002</v>
       </c>
-      <c r="B113" s="42" t="s">
+      <c r="B116" s="42" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="28">
+      <c r="E116" s="42"/>
+      <c r="G116">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="28">
         <v>32082.515513599999</v>
       </c>
-      <c r="B114" s="42" t="s">
+      <c r="B117" s="42" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="28">
+      <c r="E117" s="42"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E118" s="42"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="28">
         <v>35642.5160798</v>
       </c>
-      <c r="B116" s="42" t="s">
+      <c r="B119" s="42" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="28">
+      <c r="E119" s="42"/>
+      <c r="G119">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="28">
         <v>31807.078489299998</v>
       </c>
-      <c r="B117" s="42" t="s">
+      <c r="B120" s="42" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="28">
+      <c r="E120" s="42"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="28">
         <v>34377.592782599997</v>
       </c>
-      <c r="B119" s="42" t="s">
+      <c r="B122" s="42" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="28">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="28">
         <v>31385.698520900001</v>
       </c>
-      <c r="B120" s="42" t="s">
+      <c r="B123" s="42" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="28">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="28">
         <v>34258.6779025</v>
       </c>
-      <c r="B122" s="42" t="s">
+      <c r="B125" s="42" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="28">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="28">
         <v>31402.082680899999</v>
       </c>
-      <c r="B123" s="42" t="s">
+      <c r="B126" s="42" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="28" t="s">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="28" t="s">
         <v>487</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="28">
-        <v>36372.76</v>
-      </c>
-      <c r="B126" s="42" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="28">
-        <v>32280.05</v>
-      </c>
-      <c r="B127" s="42" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="28">
-        <v>36186.76</v>
+        <v>36372.76</v>
       </c>
       <c r="B129" s="42" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="28">
-        <v>32174.880000000001</v>
+        <v>32280.05</v>
       </c>
       <c r="B130" s="42" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="28">
-        <v>35970.25</v>
+        <v>36186.76</v>
       </c>
       <c r="B132" s="42" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="28">
-        <v>32031.05</v>
+        <v>32174.880000000001</v>
       </c>
       <c r="B133" s="42" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="28">
-        <v>35702.36</v>
+        <v>35970.25</v>
       </c>
       <c r="B135" s="42" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="28">
-        <v>31859.56</v>
+        <v>32031.05</v>
       </c>
       <c r="B136" s="42" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="28">
-        <v>35477.760000000002</v>
+        <v>35702.36</v>
       </c>
       <c r="B138" s="42" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="28">
-        <v>31723.99</v>
+        <v>31859.56</v>
       </c>
       <c r="B139" s="42" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="28">
-        <v>35101.279999999999</v>
+        <v>35477.760000000002</v>
       </c>
       <c r="B141" s="42" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="28">
-        <v>31592.21</v>
+        <v>31723.99</v>
       </c>
       <c r="B142" s="42" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="28">
-        <v>34734.089999999997</v>
+        <v>35101.279999999999</v>
       </c>
       <c r="B144" s="42" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="28">
+        <v>31592.21</v>
+      </c>
+      <c r="B145" s="42" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="28">
+        <v>34734.089999999997</v>
+      </c>
+      <c r="B147" s="42" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="28">
         <v>31479.83</v>
       </c>
-      <c r="B145" s="42" t="s">
+      <c r="B148" s="42" t="s">
         <v>511</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="28" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="28" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="28" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="28" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="28" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="28" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="28" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="28" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="28" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="28" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="28" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="28" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="28" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="28" t="s">
         <v>526</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="28" t="s">
+        <v>544</v>
+      </c>
+      <c r="B164" s="42" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="28" t="s">
+        <v>546</v>
+      </c>
+      <c r="B165" s="42" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="28">
+        <v>40532.2757413</v>
+      </c>
+      <c r="B166" s="42" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="28">
+        <v>32649.741543799999</v>
+      </c>
+      <c r="B167" s="42" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="28">
+        <v>39590.876380399997</v>
+      </c>
+      <c r="B169" s="42" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="28">
+        <v>32482.380007700001</v>
+      </c>
+      <c r="B170" s="42" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="28">
+        <v>38501.4283154</v>
+      </c>
+      <c r="B172" s="42" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="28">
+        <v>32089.951655299999</v>
+      </c>
+      <c r="B173" s="42" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="28">
+        <v>38058.538523000003</v>
+      </c>
+      <c r="B175" s="42" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="28">
+        <v>31970.810215199999</v>
+      </c>
+      <c r="B176" s="42" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="28">
+        <v>43096.791007599997</v>
+      </c>
+      <c r="B178" s="42" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="28">
+        <v>33604.025064699999</v>
+      </c>
+      <c r="B179" s="42" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="28">
+        <v>37122.373530099998</v>
+      </c>
+      <c r="B181" s="42" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="28">
+        <v>31667.560614900001</v>
+      </c>
+      <c r="B182" s="42" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="28">
+        <v>35705.505176799998</v>
+      </c>
+      <c r="B184" s="42" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="28">
+        <v>31239.412582500001</v>
+      </c>
+      <c r="B185" s="42" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="28">
+        <v>34512.7804397</v>
+      </c>
+      <c r="B188" s="28">
+        <v>103.89183869999999</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="28">
+        <v>30864.168038200001</v>
+      </c>
+      <c r="B189" s="28">
+        <v>1.2953984000000001</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="28" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="28">
+        <v>30576.4513592</v>
+      </c>
+      <c r="B192" s="42" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="28">
+        <v>39785.026074499998</v>
+      </c>
+      <c r="B193" s="42" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="28">
+        <v>30742.867327299999</v>
+      </c>
+      <c r="B195" s="42" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="28">
+        <v>39020.313529799998</v>
+      </c>
+      <c r="B196" s="42" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="28" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="28">
+        <v>30777.594452199999</v>
+      </c>
+      <c r="B199" s="42" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="28">
+        <v>39888.679278600001</v>
+      </c>
+      <c r="B200" s="42" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="28">
+        <v>30832.0437322</v>
+      </c>
+      <c r="B202" s="42" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="28">
+        <v>39694.078958400001</v>
+      </c>
+      <c r="B203" s="42" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="28">
+        <v>31082.8658765</v>
+      </c>
+      <c r="B205" s="42" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="28">
+        <v>39095.1092938</v>
+      </c>
+      <c r="B206" s="42" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="28" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="28" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="28">
+        <v>38163.228498199998</v>
+      </c>
+      <c r="B211" s="28" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="28">
+        <v>32629.488922100001</v>
+      </c>
+      <c r="B212" s="28" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="28">
+        <v>38060.19</v>
+      </c>
+      <c r="B214" s="42" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="28">
+        <v>32739.54</v>
+      </c>
+      <c r="B215" s="42" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="28">
+        <v>37703.629999999997</v>
+      </c>
+      <c r="B217" s="42" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="28">
+        <v>32631.88</v>
+      </c>
+      <c r="B218" s="42" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="28">
+        <v>37215.75</v>
+      </c>
+      <c r="B220" s="42" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="28">
+        <v>32450.71</v>
+      </c>
+      <c r="B221" s="42" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="28">
+        <v>36791.79</v>
+      </c>
+      <c r="B223" s="42" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="28">
+        <v>32364.92</v>
+      </c>
+      <c r="B224" s="42" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" s="28">
+        <v>36372.76</v>
+      </c>
+      <c r="B226" s="42" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" s="28">
+        <v>32280.05</v>
+      </c>
+      <c r="B227" s="42" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="28">
+        <v>36186.76</v>
+      </c>
+      <c r="B229" s="42" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" s="28">
+        <v>32174.880000000001</v>
+      </c>
+      <c r="B230" s="42" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" s="28">
+        <v>35970.25</v>
+      </c>
+      <c r="B232" s="42" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" s="28">
+        <v>32031.05</v>
+      </c>
+      <c r="B233" s="42" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="28">
+        <v>35702.36</v>
+      </c>
+      <c r="B235" s="42" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="28">
+        <v>31859.56</v>
+      </c>
+      <c r="B236" s="42" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" s="28">
+        <v>35477.760000000002</v>
+      </c>
+      <c r="B238" s="42" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" s="28">
+        <v>31723.99</v>
+      </c>
+      <c r="B239" s="42" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="28">
+        <v>35101.279999999999</v>
+      </c>
+      <c r="B241" s="42" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" s="28">
+        <v>31592.21</v>
+      </c>
+      <c r="B242" s="42" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" s="28">
+        <v>34734.089999999997</v>
+      </c>
+      <c r="B244" s="42" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" s="28">
+        <v>31479.83</v>
+      </c>
+      <c r="B245" s="42" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="28">
+        <v>34065.42</v>
+      </c>
+      <c r="B247" s="42" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="28">
+        <v>31457.71</v>
+      </c>
+      <c r="B248" s="42" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="28" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="59">
+        <v>30451.992083900001</v>
+      </c>
+      <c r="B251" s="59">
+        <v>103.8553513</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="59">
+        <v>39770.158830499997</v>
+      </c>
+      <c r="B252" s="59">
+        <v>1.3759417</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="59"/>
+      <c r="B253" s="59"/>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" s="59">
+        <v>31328.920852700001</v>
+      </c>
+      <c r="B254" s="59">
+        <v>103.8632314</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" s="59">
+        <v>39969.945966599997</v>
+      </c>
+      <c r="B255" s="59">
+        <v>1.3777482999999999</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" s="59"/>
+      <c r="B256" s="59"/>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" s="59">
+        <v>31499.1505488</v>
+      </c>
+      <c r="B257" s="59">
+        <v>103.86476089999999</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" s="59">
+        <v>39170.2856139</v>
+      </c>
+      <c r="B258" s="59">
+        <v>1.3705164999999999</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" s="59"/>
+      <c r="B259" s="59"/>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" s="59">
+        <v>30690.992468100001</v>
+      </c>
+      <c r="B260" s="59">
+        <v>103.857499</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="59">
+        <v>39019.5417418</v>
+      </c>
+      <c r="B261" s="59">
+        <v>1.3691533</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" s="59"/>
+      <c r="B262" s="59"/>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="59">
+        <v>30814.207316200002</v>
+      </c>
+      <c r="B263" s="59">
+        <v>103.85860630000001</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="59">
+        <v>39781.755438499997</v>
+      </c>
+      <c r="B264" s="59">
+        <v>1.3760463000000001</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" s="59"/>
+      <c r="B265" s="59"/>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" s="59">
+        <v>31063.382612400001</v>
+      </c>
+      <c r="B266" s="59">
+        <v>103.8608452</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" s="59">
+        <v>39106.710509800003</v>
+      </c>
+      <c r="B267" s="59">
+        <v>1.3699416</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" s="28" t="s">
+        <v>593</v>
+      </c>
+      <c r="B269" s="42" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="B270" s="42" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" s="28" t="s">
+        <v>594</v>
+      </c>
+      <c r="B271" s="42" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" s="28" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" s="28">
+        <v>30790.9181002</v>
+      </c>
+      <c r="B273" s="59">
+        <v>103.8583969</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" s="28">
+        <v>38176.531180999998</v>
+      </c>
+      <c r="B274" s="59">
+        <v>1.3615294</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" s="28" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" s="28">
+        <v>30767.915796199999</v>
+      </c>
+      <c r="B277" s="59">
+        <v>103.8581904</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" s="28">
+        <v>40638.217391300001</v>
+      </c>
+      <c r="B278" s="59">
+        <v>1.3837919999999999</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="28" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="28">
+        <v>30735.826324099999</v>
+      </c>
+      <c r="B281" s="42" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="28">
+        <v>36911.550443799999</v>
+      </c>
+      <c r="B282" s="42" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" s="28" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="28">
+        <v>30332.467923699998</v>
+      </c>
+      <c r="B285" s="42" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" s="28">
+        <v>37788.599724599997</v>
+      </c>
+      <c r="B286" s="42" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" s="28" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" s="28">
+        <v>31214.9684046</v>
+      </c>
+      <c r="B289" s="42" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" s="28">
+        <v>37351.410860199998</v>
+      </c>
+      <c r="B290" s="42" t="s">
+        <v>603</v>
       </c>
     </row>
   </sheetData>
@@ -6689,7 +9300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -6790,7 +9401,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6862,10 +9473,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C143"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="C144" sqref="C144"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -7577,6 +10188,24 @@
         <v>536</v>
       </c>
     </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="47" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="47" t="s">
+        <v>540</v>
+      </c>
+      <c r="C146" s="47" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C147" s="47" t="s">
+        <v>542</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7588,8 +10217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -7877,23 +10506,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e39e7e9e36de66d473ce04bb4ab2dbb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19dc5994665da46609c24125788630d8" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -8098,32 +10710,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EFB9284-2381-45C4-9342-D2A846659864}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C78C4875-2E31-4ACC-AEED-0DAFD072C30B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8140,4 +10744,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EFB9284-2381-45C4-9342-D2A846659864}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AB413C-A07F-4EE8-909C-4B888D55CBB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>